<commit_message>
RDCC-2215: Updated the test cases.
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsxWithData.xlsx
+++ b/src/test/resources/xlsxWithData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/rd-caseworker-ref-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC368C7-266A-9944-ABDB-2467BE01F45C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB89764-CF95-C949-81C2-A15E4CB990C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8928,7 +8928,7 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>